<commit_message>
tweaked MMD json data, and css
</commit_message>
<xml_diff>
--- a/appendix_changes.xlsx
+++ b/appendix_changes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>MMD</t>
   </si>
@@ -69,10 +69,6 @@
     <t>Title: Gender diversity at Global Voices</t>
   </si>
   <si>
-    <t>Title: 
-The humanitarian fallout of the conflict in Syria reaches new proportions as the number of estimated refugees reaches one million. Who's Helping?</t>
-  </si>
-  <si>
     <t>Title: Percentage of people trusting various components that comprise the Financial Trust Index.</t>
   </si>
   <si>
@@ -94,14 +90,26 @@
     <t>"(See Glossary.)"</t>
   </si>
   <si>
-    <t>Should 74, 75, 76 be title?</t>
+    <t>Text: The idea that hard work leads to material success is no longer, if it ever was, a uniquely Western value.</t>
+  </si>
+  <si>
+    <t>Text: The Pew Forum survey included several questions designed to probe the kinds of requests that inmates make for accommodation of their religious beliefs and practices, as well as the frequency with which they are granted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text: Two years after nationwide protests sparked upheaval in Syria, the ensuing refugee crisis has reached one million people. </t>
+  </si>
+  <si>
+    <t>Text-end: The British charity Save the Children claims that many of these children have been separated from one or both of their parents.</t>
+  </si>
+  <si>
+    <t>Title: The humanitarian fallout of the conflict in Syria reaches new proportions as the number of estimated refugees reaches one million. Who's Helping?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,14 +121,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -181,17 +181,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,7 +499,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,10 +514,10 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -529,10 +532,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -574,12 +577,15 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>9</v>
       </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>60</v>
       </c>
       <c r="D8" t="s">
@@ -605,7 +611,7 @@
       <c r="A12" s="4">
         <v>66</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -636,12 +642,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>74</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,12 +655,15 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -662,7 +671,7 @@
         <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -670,38 +679,57 @@
         <v>68</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="9">
         <v>73</v>
       </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>75</v>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
+        <v>75</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="9" t="s">
+      <c r="D24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
         <v>22</v>
       </c>
-      <c r="D25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>25</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added titles and formatting to MMDs
</commit_message>
<xml_diff>
--- a/appendix_changes.xlsx
+++ b/appendix_changes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="9525"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="21075" windowHeight="9465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>MMD</t>
   </si>
@@ -36,21 +36,6 @@
     <t>18+19</t>
   </si>
   <si>
-    <t>Text: Mutual fund investors poured some $17 billion into domestic equity funds in January, reversing 2012’s trend, according to the Investment Company Institute (ICI), an industry trade group</t>
-  </si>
-  <si>
-    <t>Text: In the wake of four years of economic turmoil around the world and political upheaval in a number of nations, very few people are satisfied with the way things are going in their country.</t>
-  </si>
-  <si>
-    <t>Title: Few Better Off Than Five Years Ago</t>
-  </si>
-  <si>
-    <t>Title: Nonmedical Use of Adderall®, by College Enrollment Status</t>
-  </si>
-  <si>
-    <t>Text: Asian Americans trace their roots to any of dozens of countries in the Far East, Southeast Asia and the Indian subcontinent. Each country of origin subgroup has its own unique history, culture, language, religious beliefs, economic and demographic traits, social and political values, and pathways into America.</t>
-  </si>
-  <si>
     <t>Removed text?</t>
   </si>
   <si>
@@ -66,59 +51,110 @@
     <t>Title: Asians in the U.S. and in Asia</t>
   </si>
   <si>
-    <t>Title: Gender diversity at Global Voices</t>
-  </si>
-  <si>
-    <t>Title: Percentage of people trusting various components that comprise the Financial Trust Index.</t>
-  </si>
-  <si>
     <t>Title: The Rise of Asian Americans</t>
   </si>
   <si>
     <t>Text: Is it possible that David Cameron's Britain is a colder place than Tony Blair's? Or one with less sunshine? Well, maybe.</t>
   </si>
   <si>
-    <t>Text: The Pew Forum survey asked chaplains to rate the prevalence of extremist views among inmates in each of 12 religious groups. A majority of respondents to this question say that religious extremism is either very common (22%) or somewhat common (36%) among Muslim inmates (including followers of the Nation of Islam and the Moorish Science Temple of America).</t>
-  </si>
-  <si>
-    <t>NOTES:</t>
-  </si>
-  <si>
-    <t>3 has a new reference</t>
-  </si>
-  <si>
     <t>"(See Glossary.)"</t>
   </si>
   <si>
-    <t>Text: The idea that hard work leads to material success is no longer, if it ever was, a uniquely Western value.</t>
-  </si>
-  <si>
-    <t>Text: The Pew Forum survey included several questions designed to probe the kinds of requests that inmates make for accommodation of their religious beliefs and practices, as well as the frequency with which they are granted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Text: Two years after nationwide protests sparked upheaval in Syria, the ensuing refugee crisis has reached one million people. </t>
-  </si>
-  <si>
-    <t>Text-end: The British charity Save the Children claims that many of these children have been separated from one or both of their parents.</t>
-  </si>
-  <si>
     <t>Title: The humanitarian fallout of the conflict in Syria reaches new proportions as the number of estimated refugees reaches one million. Who's Helping?</t>
   </si>
   <si>
     <t>Other changes</t>
   </si>
   <si>
-    <t>% added to Y axis on graph</t>
-  </si>
-  <si>
     <t>NEED TO ADD REF</t>
+  </si>
+  <si>
+    <t>%' symbol added to Y axis on graph</t>
+  </si>
+  <si>
+    <t>Removed, Viz is pre-highlighted</t>
+  </si>
+  <si>
+    <t>Bad Viz. Removed</t>
+  </si>
+  <si>
+    <t>Sub-optimal Encoding of Viz. Removed</t>
+  </si>
+  <si>
+    <t>Confusing MMD. Removed</t>
+  </si>
+  <si>
+    <t>"and median household wealth ($83,500 vs. $68,529)." (not a reference)</t>
+  </si>
+  <si>
+    <t>Fix Viz from Source</t>
+  </si>
+  <si>
+    <t>Removed hyperlinks from bottom of viz .png</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Religion in Prisons – A 50-State Survey of Prison Chaplains</t>
+  </si>
+  <si>
+    <t>Boomers Still Cautious About Stocks</t>
+  </si>
+  <si>
+    <t>Pervasive Gloom About the World Economy</t>
+  </si>
+  <si>
+    <t>The Pew Forum survey asked chaplains to rate the prevalence of extremist views among inmates in each of 12 religious groups. A majority of respondents to this question say that religious extremism is either very common (22%) or somewhat common (36%) among Muslim inmates (including followers of the Nation of Islam and the Moorish Science Temple of America).</t>
+  </si>
+  <si>
+    <t>Mutual fund investors poured some $17 billion into domestic equity funds in January, reversing 2012’s trend, according to the Investment Company Institute (ICI), an industry trade group</t>
+  </si>
+  <si>
+    <t>In the wake of four years of economic turmoil around the world and political upheaval in a number of nations, very few people are satisfied with the way things are going in their country.</t>
+  </si>
+  <si>
+    <t>The Pew Forum survey included several questions designed to probe the kinds of requests that inmates make for accommodation of their religious beliefs and practices, as well as the frequency with which they are granted.</t>
+  </si>
+  <si>
+    <t>Nonmedical Use of Adderall®, by College Enrollment Status</t>
+  </si>
+  <si>
+    <t>The Rise of Asian Americans</t>
+  </si>
+  <si>
+    <t>Asian Americans trace their roots to any of dozens of countries in the Far East, Southeast Asia and the Indian subcontinent. Each country of origin subgroup has its own unique history, culture, language, religious beliefs, economic and demographic traits, social and political values, and pathways into America.</t>
+  </si>
+  <si>
+    <t>Gender diversity at Global Voices</t>
+  </si>
+  <si>
+    <t>Syrian refugees: how many are there and where are they?</t>
+  </si>
+  <si>
+    <t>The humanitarian fallout of the conflict in Syria reaches new proportions as the number of estimated refugees reaches one million. Who's Helping?</t>
+  </si>
+  <si>
+    <t>The idea that hard work leads to material success is no longer, if it ever was, a uniquely Western value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two years after nationwide protests sparked upheaval in Syria, the ensuing refugee crisis has reached one million people. </t>
+  </si>
+  <si>
+    <t>End: The British charity Save the Children claims that many of these children have been separated from one or both of their parents.</t>
+  </si>
+  <si>
+    <t>Percentage of people trusting various components that comprise the Financial Trust Index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +181,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -213,7 +257,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,245 +580,371 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="164.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="164.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="18">
+        <v>40990</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="18">
+        <v>40990</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="18">
+        <v>41324</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="18">
+        <v>41102</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="18">
+        <v>41102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="18">
+        <v>40990</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>60</v>
       </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="18">
+        <v>39910</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="18">
+        <v>39910</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="18">
+        <v>39910</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="18">
+        <v>41079</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>66</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="18">
+        <v>41079</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>77</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>77</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>70</v>
       </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>72</v>
       </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="18">
+        <v>41341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>74</v>
       </c>
+      <c r="C16" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F16" s="18">
+        <v>41339</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>11</v>
       </c>
-      <c r="E17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="18">
+        <v>41212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>30</v>
       </c>
-      <c r="E18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="E18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="18">
+        <v>41102</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
         <v>65</v>
       </c>
-      <c r="E19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
         <v>68</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>73</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="11"/>
-      <c r="E21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="17"/>
+      <c r="D21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="18">
+        <v>41339</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="11"/>
-      <c r="E22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="C22" s="17"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="9"/>
+      <c r="G22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
         <v>75</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>76</v>
       </c>
+      <c r="D24" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="E24" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" t="s">
-        <v>22</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F24" s="18">
+        <v>41339</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>